<commit_message>
Added gene symbol to riGenerateTestData. Tweaked asciidoc to create web page from .adoc files.
</commit_message>
<xml_diff>
--- a/ri-generate/src/test/resources/riGenerateTestData.xlsx
+++ b/ri-generate/src/test/resources/riGenerateTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrelac/sql/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrelac/workspace/ri/ri-generate/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="6760" windowWidth="39060" windowHeight="15020" tabRatio="500"/>
+    <workbookView xWindow="8540" yWindow="6080" windowWidth="33680" windowHeight="14120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="gene_sent1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/mrelac/workspace/ri/ri-generate/gene_sent1.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/mrelac/workspace/ri/ri-generate/gene_sent1.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="103">
   <si>
     <t>withdrawn</t>
   </si>
@@ -413,13 +413,52 @@
 The MPI2 (KOMP2) informatics consortium
 </t>
   </si>
+  <si>
+    <t>Gene Symbol</t>
+  </si>
+  <si>
+    <t>gene-010</t>
+  </si>
+  <si>
+    <t>gene-020</t>
+  </si>
+  <si>
+    <t>gene-030</t>
+  </si>
+  <si>
+    <t>gene-040</t>
+  </si>
+  <si>
+    <t>gene-050</t>
+  </si>
+  <si>
+    <t>gene-060</t>
+  </si>
+  <si>
+    <t>gene-070</t>
+  </si>
+  <si>
+    <t>gene-080</t>
+  </si>
+  <si>
+    <t>gene-090</t>
+  </si>
+  <si>
+    <t>gene-100</t>
+  </si>
+  <si>
+    <t>gene-110</t>
+  </si>
+  <si>
+    <t>gene-120</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -480,13 +519,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -768,211 +807,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.5" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="2.1640625" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" customWidth="1"/>
-    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="1" max="2" width="54.5" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="2" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="2.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>43</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>44</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>20</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="L9" s="1" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>49</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>50</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>37</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>5</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>8</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>7</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>9</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
         <v>14</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -980,8 +1020,8 @@
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="L11" t="s">
-        <v>36</v>
+      <c r="K11">
+        <v>1</v>
       </c>
       <c r="M11" t="s">
         <v>36</v>
@@ -995,44 +1035,47 @@
       <c r="P11" t="s">
         <v>36</v>
       </c>
-      <c r="S11">
+      <c r="Q11" t="s">
+        <v>36</v>
+      </c>
+      <c r="T11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>14</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="L12" t="s">
-        <v>36</v>
-      </c>
       <c r="M12" t="s">
         <v>36</v>
       </c>
@@ -1045,43 +1088,46 @@
       <c r="P12" t="s">
         <v>36</v>
       </c>
-      <c r="S12">
+      <c r="Q12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
         <v>16</v>
       </c>
       <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
         <v>14</v>
       </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
       <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="L13" t="s">
-        <v>36</v>
+      <c r="K13">
+        <v>3</v>
       </c>
       <c r="M13" t="s">
         <v>36</v>
@@ -1095,519 +1141,549 @@
       <c r="P13" t="s">
         <v>36</v>
       </c>
-      <c r="S13">
+      <c r="Q13" t="s">
+        <v>36</v>
+      </c>
+      <c r="T13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>2.1</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>3.1</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>6.1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="H14">
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14">
         <v>4</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>4</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>4</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>18</v>
       </c>
-      <c r="N14" t="s">
-        <v>36</v>
-      </c>
       <c r="O14" t="s">
         <v>36</v>
       </c>
       <c r="P14" t="s">
         <v>36</v>
       </c>
-      <c r="S14">
+      <c r="Q14" t="s">
+        <v>36</v>
+      </c>
+      <c r="T14">
         <v>1.2</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>2.1</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="H15">
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15">
         <v>5</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>5</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>5</v>
       </c>
-      <c r="M15" t="s">
-        <v>12</v>
-      </c>
       <c r="N15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" t="s">
         <v>13</v>
       </c>
-      <c r="O15" t="s">
-        <v>36</v>
-      </c>
       <c r="P15" t="s">
         <v>36</v>
       </c>
-      <c r="S15">
+      <c r="Q15" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15">
         <v>1.2</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>2.1</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>5.2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>6</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>2</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>6</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>6</v>
       </c>
-      <c r="M16" t="s">
-        <v>12</v>
-      </c>
       <c r="N16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" t="s">
         <v>16</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>17</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>14</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>1.2</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>2.1</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>6.1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>15</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>7</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>7</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>7</v>
       </c>
-      <c r="M17" t="s">
-        <v>12</v>
-      </c>
       <c r="N17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" t="s">
         <v>16</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>13</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>15</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>1.2</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>2.1</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>4.2</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>6.2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>2</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>8</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>8</v>
       </c>
-      <c r="M18" t="s">
-        <v>12</v>
-      </c>
       <c r="N18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O18" t="s">
         <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>36</v>
-      </c>
-      <c r="S18">
+        <v>17</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18">
         <v>1.2</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>2.1</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>5.2</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>16</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>9</v>
       </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
       <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
         <v>9</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>9</v>
       </c>
-      <c r="M19" t="s">
-        <v>12</v>
-      </c>
       <c r="N19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O19" t="s">
         <v>17</v>
       </c>
       <c r="P19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S19">
+        <v>17</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19">
         <v>1.2</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>2.1</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>4.2</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>14</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>10</v>
       </c>
-      <c r="I20">
-        <v>3</v>
-      </c>
       <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
         <v>10</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>10</v>
       </c>
-      <c r="M20" t="s">
-        <v>12</v>
-      </c>
       <c r="N20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" t="s">
         <v>17</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>13</v>
       </c>
-      <c r="P20" t="s">
-        <v>36</v>
-      </c>
-      <c r="S20">
+      <c r="Q20" t="s">
+        <v>36</v>
+      </c>
+      <c r="T20">
         <v>1.2</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>2.1</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>4.0999999999999996</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>5.2</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>6.1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>14</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>11</v>
       </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
       <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
         <v>11</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>11</v>
       </c>
-      <c r="M21" t="s">
-        <v>12</v>
-      </c>
       <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21" t="s">
         <v>13</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>17</v>
       </c>
-      <c r="P21" t="s">
-        <v>36</v>
-      </c>
-      <c r="S21">
+      <c r="Q21" t="s">
+        <v>36</v>
+      </c>
+      <c r="T21">
         <v>1.2</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>2.1</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>4.2</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>6.1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>14</v>
       </c>
-      <c r="H23">
-        <v>12</v>
-      </c>
       <c r="I23">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J23">
-        <v>12</v>
-      </c>
-      <c r="L23">
-        <v>12</v>
-      </c>
-      <c r="M23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>12</v>
+      </c>
+      <c r="M23">
         <v>12</v>
       </c>
       <c r="N23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" t="s">
         <v>13</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>17</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>14</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="I9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1629,9 +1705,9 @@
     <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.6640625" customWidth="1"/>
     <col min="11" max="11" width="106" customWidth="1"/>
   </cols>
@@ -1655,13 +1731,13 @@
       <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="J1" t="s">
@@ -1690,16 +1766,16 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>42915.705459293982</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>42915.705459421297</v>
       </c>
       <c r="J2" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1722,16 +1798,16 @@
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>42915.705459525459</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>42915.705459548612</v>
       </c>
       <c r="J3" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1748,16 +1824,16 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>42915.705459560188</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>42915.705459571756</v>
       </c>
       <c r="J4" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1774,16 +1850,16 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J5" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1800,16 +1876,16 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J6" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1829,16 +1905,16 @@
       <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J7" t="s">
         <v>65</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1858,16 +1934,16 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J8" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1887,16 +1963,16 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J9" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1916,16 +1992,16 @@
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J10" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1948,16 +2024,16 @@
       <c r="F11">
         <v>5</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J11" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1980,16 +2056,16 @@
       <c r="F12">
         <v>5</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J12" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2000,16 +2076,16 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>42915.705434629628</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>42915.705434791664</v>
       </c>
       <c r="J13" t="s">
         <v>88</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tidied up email text snippets. Standardised test data xml files.
</commit_message>
<xml_diff>
--- a/ri-generate/src/test/resources/riGenerateTestData.xlsx
+++ b/ri-generate/src/test/resources/riGenerateTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="6080" windowWidth="33680" windowHeight="14120" tabRatio="500"/>
+    <workbookView xWindow="5480" yWindow="11720" windowWidth="41400" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="2" r:id="rId1"/>
@@ -809,7 +809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -879,7 +881,7 @@
         <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Fixed Register Interest validation rule and tweaked data.
</commit_message>
<xml_diff>
--- a/ri-generate/src/test/resources/riGenerateTestData.xlsx
+++ b/ri-generate/src/test/resources/riGenerateTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54680" yWindow="3980" windowWidth="42980" windowHeight="22560" tabRatio="500"/>
+    <workbookView xWindow="59940" yWindow="2360" windowWidth="42980" windowHeight="22560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="2" r:id="rId1"/>
@@ -696,7 +696,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -707,6 +707,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -717,17 +718,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1027,7 +1018,7 @@
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1314,7 +1305,7 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U14" s="5">
         <v>1.2</v>
@@ -1613,13 +1604,13 @@
       <c r="O19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="P19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="Q19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="S19" s="5"/>
@@ -1681,16 +1672,16 @@
       <c r="O20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P20" s="5" t="s">
+      <c r="P20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="5"/>
+      <c r="Q20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S20" s="6"/>
       <c r="T20" s="5" t="s">
         <v>1</v>
       </c>
@@ -1747,16 +1738,16 @@
       <c r="O21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P21" s="5" t="s">
+      <c r="P21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="5"/>
+      <c r="Q21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="6"/>
       <c r="T21" s="5" t="s">
         <v>1</v>
       </c>
@@ -1815,16 +1806,16 @@
       <c r="O22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q22" s="5" t="s">
+      <c r="P22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="5"/>
+      <c r="Q22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="6"/>
       <c r="T22" s="5" t="s">
         <v>1</v>
       </c>
@@ -1883,16 +1874,16 @@
       <c r="O23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="5" t="s">
+      <c r="P23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q23" s="5" t="s">
+      <c r="Q23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="S23" s="5"/>
+      <c r="R23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S23" s="6"/>
       <c r="T23" s="5" t="s">
         <v>1</v>
       </c>
@@ -1953,16 +1944,16 @@
       <c r="O24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P24" s="5" t="s">
+      <c r="P24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="Q24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S24" s="5"/>
+      <c r="R24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S24" s="6"/>
       <c r="T24" s="5" t="s">
         <v>1</v>
       </c>
@@ -5601,7 +5592,7 @@
       <c r="Z96" s="5"/>
       <c r="AA96" s="5"/>
     </row>
-    <row r="97" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
@@ -5628,7 +5619,7 @@
       <c r="Z97" s="5"/>
       <c r="AA97" s="5"/>
     </row>
-    <row r="98" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
@@ -5655,7 +5646,7 @@
       <c r="Z98" s="5"/>
       <c r="AA98" s="5"/>
     </row>
-    <row r="99" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
@@ -5682,7 +5673,7 @@
       <c r="Z99" s="5"/>
       <c r="AA99" s="5"/>
     </row>
-    <row r="100" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -5709,7 +5700,7 @@
       <c r="Z100" s="5"/>
       <c r="AA100" s="5"/>
     </row>
-    <row r="101" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
@@ -5736,7 +5727,10 @@
       <c r="Z101" s="5"/>
       <c r="AA101" s="5"/>
     </row>
-    <row r="102" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B102" s="4">
+        <v>10</v>
+      </c>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
@@ -5763,7 +5757,10 @@
       <c r="Z102" s="5"/>
       <c r="AA102" s="5"/>
     </row>
-    <row r="103" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B103" s="4">
+        <v>30</v>
+      </c>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
@@ -5790,7 +5787,10 @@
       <c r="Z103" s="5"/>
       <c r="AA103" s="5"/>
     </row>
-    <row r="104" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B104" s="4">
+        <v>40</v>
+      </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
@@ -5817,7 +5817,10 @@
       <c r="Z104" s="5"/>
       <c r="AA104" s="5"/>
     </row>
-    <row r="105" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B105" s="4">
+        <v>50</v>
+      </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
@@ -5844,7 +5847,10 @@
       <c r="Z105" s="5"/>
       <c r="AA105" s="5"/>
     </row>
-    <row r="106" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B106" s="4">
+        <v>60</v>
+      </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
@@ -5871,7 +5877,10 @@
       <c r="Z106" s="5"/>
       <c r="AA106" s="5"/>
     </row>
-    <row r="107" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B107" s="4">
+        <v>70</v>
+      </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
@@ -5898,7 +5907,10 @@
       <c r="Z107" s="5"/>
       <c r="AA107" s="5"/>
     </row>
-    <row r="108" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B108" s="4">
+        <v>80</v>
+      </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
@@ -5925,7 +5937,10 @@
       <c r="Z108" s="5"/>
       <c r="AA108" s="5"/>
     </row>
-    <row r="109" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B109" s="4">
+        <v>90</v>
+      </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
@@ -5952,7 +5967,10 @@
       <c r="Z109" s="5"/>
       <c r="AA109" s="5"/>
     </row>
-    <row r="110" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B110" s="4">
+        <v>100</v>
+      </c>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
       <c r="E110" s="5"/>
@@ -5979,7 +5997,10 @@
       <c r="Z110" s="5"/>
       <c r="AA110" s="5"/>
     </row>
-    <row r="111" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B111" s="4">
+        <v>110</v>
+      </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
@@ -6006,7 +6027,10 @@
       <c r="Z111" s="5"/>
       <c r="AA111" s="5"/>
     </row>
-    <row r="112" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B112" s="4">
+        <v>120</v>
+      </c>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
@@ -6033,7 +6057,10 @@
       <c r="Z112" s="5"/>
       <c r="AA112" s="5"/>
     </row>
-    <row r="113" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B113" s="4">
+        <v>130</v>
+      </c>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
@@ -6060,7 +6087,10 @@
       <c r="Z113" s="5"/>
       <c r="AA113" s="5"/>
     </row>
-    <row r="114" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B114" s="4">
+        <v>140</v>
+      </c>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
@@ -6087,7 +6117,10 @@
       <c r="Z114" s="5"/>
       <c r="AA114" s="5"/>
     </row>
-    <row r="115" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B115" s="4">
+        <v>150</v>
+      </c>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
       <c r="E115" s="5"/>
@@ -6114,7 +6147,10 @@
       <c r="Z115" s="5"/>
       <c r="AA115" s="5"/>
     </row>
-    <row r="116" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B116" s="4">
+        <v>160</v>
+      </c>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
@@ -6141,7 +6177,10 @@
       <c r="Z116" s="5"/>
       <c r="AA116" s="5"/>
     </row>
-    <row r="117" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B117" s="4">
+        <v>170</v>
+      </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
@@ -6168,7 +6207,10 @@
       <c r="Z117" s="5"/>
       <c r="AA117" s="5"/>
     </row>
-    <row r="118" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B118" s="4">
+        <v>180</v>
+      </c>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
@@ -6195,7 +6237,10 @@
       <c r="Z118" s="5"/>
       <c r="AA118" s="5"/>
     </row>
-    <row r="119" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B119" s="4">
+        <v>190</v>
+      </c>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
@@ -6222,7 +6267,10 @@
       <c r="Z119" s="5"/>
       <c r="AA119" s="5"/>
     </row>
-    <row r="120" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B120" s="4">
+        <v>200</v>
+      </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
@@ -6249,7 +6297,10 @@
       <c r="Z120" s="5"/>
       <c r="AA120" s="5"/>
     </row>
-    <row r="121" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B121" s="4">
+        <v>210</v>
+      </c>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
@@ -6276,7 +6327,10 @@
       <c r="Z121" s="5"/>
       <c r="AA121" s="5"/>
     </row>
-    <row r="122" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B122" s="4">
+        <v>220</v>
+      </c>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
@@ -6303,7 +6357,7 @@
       <c r="Z122" s="5"/>
       <c r="AA122" s="5"/>
     </row>
-    <row r="123" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
@@ -6330,7 +6384,7 @@
       <c r="Z123" s="5"/>
       <c r="AA123" s="5"/>
     </row>
-    <row r="124" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
@@ -6357,7 +6411,7 @@
       <c r="Z124" s="5"/>
       <c r="AA124" s="5"/>
     </row>
-    <row r="125" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
@@ -6384,7 +6438,7 @@
       <c r="Z125" s="5"/>
       <c r="AA125" s="5"/>
     </row>
-    <row r="126" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
@@ -6411,7 +6465,7 @@
       <c r="Z126" s="5"/>
       <c r="AA126" s="5"/>
     </row>
-    <row r="127" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
@@ -6438,7 +6492,7 @@
       <c r="Z127" s="5"/>
       <c r="AA127" s="5"/>
     </row>
-    <row r="128" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
@@ -8815,9 +8869,8 @@
       <c r="AA215" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A30:Y111">
-    <sortCondition descending="1" ref="T30:T111"/>
-    <sortCondition ref="C30:C111"/>
+  <sortState ref="B102:B122">
+    <sortCondition ref="B102:B122"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="D11:H11"/>

</xml_diff>